<commit_message>
fix up comments, hyperlinks, and formulae consumption tests
</commit_message>
<xml_diff>
--- a/tests/data/10_comments_hyperlinks_formulae.xlsx
+++ b/tests/data/10_comments_hyperlinks_formulae.xlsx
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Sheet2!A1</t>
   </si>
@@ -109,13 +109,31 @@
   </si>
   <si>
     <t>Sheet2!A2</t>
+  </si>
+  <si>
+    <t>hyperlink1</t>
+  </si>
+  <si>
+    <t>hyperlink2</t>
+  </si>
+  <si>
+    <t>https://google.com/</t>
+  </si>
+  <si>
+    <t>mailto:invalid@example.com?subject=important</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +146,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,13 +173,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,48 +458,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1" t="str">
+        <f>CONCATENATE(C2,C3)</f>
+        <v>ab</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A6" location="Sheet1!A1" display="Sheet1!A1"/>
+    <hyperlink ref="A7" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <f>C2*C3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="https://apple.com/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improve hyperlinks and style round tripping
</commit_message>
<xml_diff>
--- a/tests/data/10_comments_hyperlinks_formulae.xlsx
+++ b/tests/data/10_comments_hyperlinks_formulae.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
@@ -16,11 +11,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -99,53 +89,47 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
+    <t>Sheet1!A1</t>
+  </si>
+  <si>
+    <t>Sheet1!A2</t>
+  </si>
+  <si>
+    <t>hyperlink1</t>
+  </si>
+  <si>
+    <t>https://google.com/</t>
+  </si>
+  <si>
+    <t>mailto:invalid@example.com?subject=important</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>Sheet2!A1</t>
   </si>
   <si>
-    <t>Sheet1!A1</t>
-  </si>
-  <si>
-    <t>Sheet1!A2</t>
-  </si>
-  <si>
     <t>Sheet2!A2</t>
   </si>
   <si>
-    <t>hyperlink1</t>
-  </si>
-  <si>
     <t>hyperlink2</t>
-  </si>
-  <si>
-    <t>https://google.com/</t>
-  </si>
-  <si>
-    <t>mailto:invalid@example.com?subject=important</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -175,15 +159,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -457,7 +441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -468,60 +452,59 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <f>CONCATENATE(C2,C3)</f>
-        <v>ab</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" location="Sheet1!A1" display="Sheet1!A1"/>
-    <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -532,16 +515,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1">
         <f>C2*C3</f>
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -554,14 +536,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://apple.com/"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>